<commit_message>
added EMR-5331_SubStore_PatientConsumption_CannotAbleToConsumeItem.py and added function in LibModuleProcurement.py and in LibModuleSubStore.py and change in excelTestCasesSystemTest_SNCH.xlsx
</commit_message>
<xml_diff>
--- a/Library/SystemTestExcel/excelTestCasesSystemTest_SNCH.xlsx
+++ b/Library/SystemTestExcel/excelTestCasesSystemTest_SNCH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\AutomationTest\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutomationNew\AutomationTest\Library\SystemTestExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -132,15 +132,9 @@
     <t>TC027</t>
   </si>
   <si>
-    <t>TC028</t>
-  </si>
-  <si>
     <t>ADT\TC009AdmissionDischargeTransferToBeRefund.py</t>
   </si>
   <si>
-    <t>TC029</t>
-  </si>
-  <si>
     <t>ADT\TC011AdmissionDischargeTransferNoDeposit.py</t>
   </si>
   <si>
@@ -177,9 +171,6 @@
     <t>Reports\TC008DiscountReport.py</t>
   </si>
   <si>
-    <t>TC040</t>
-  </si>
-  <si>
     <t>Reports\TC009DepositBalanceReport.py</t>
   </si>
   <si>
@@ -285,39 +276,12 @@
     <t>Failed due to old Patient</t>
   </si>
   <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>EMR-4920</t>
-  </si>
-  <si>
-    <t>Failed due to EMR-4920</t>
-  </si>
-  <si>
-    <t>Script need to maintain</t>
-  </si>
-  <si>
-    <t>Happy Path Testing</t>
-  </si>
-  <si>
-    <t>EMR-4923</t>
-  </si>
-  <si>
     <t>TC034</t>
   </si>
   <si>
     <t>TC037</t>
   </si>
   <si>
-    <t>EMR-4926</t>
-  </si>
-  <si>
-    <t>Issues and Requirement changing need to add credit organization in credit billings</t>
-  </si>
-  <si>
-    <t>Requirement changing need to add credit organization in credit billings</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Sales\TC04NarcoticDailySalesReport.py</t>
   </si>
   <si>
@@ -327,9 +291,6 @@
     <t>ADT\TC010AdmissionDischargeTransferToBePaid.py</t>
   </si>
   <si>
-    <t>ADT\TC012DischargeHappyPath.py</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Purchase\TC01ItemWisePurchaseReport.py</t>
   </si>
   <si>
@@ -342,12 +303,6 @@
     <t>Pharmacy\Reports\TC005InvoiceSaleReturnBillingReport.py</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\TC010VerifyPharmacyDashboard.py</t>
-  </si>
-  <si>
-    <t>Pharmacy\Reports\TC011VerifyStockItemsReport.py</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Purchase\TC03ReturnToSupplierReport.py</t>
   </si>
   <si>
@@ -366,9 +321,6 @@
     <t>Pharmacy\Reports\Stock\TC01SupplierStockReport.py</t>
   </si>
   <si>
-    <t>Pharmacy\Reports\Stock\TC02ExpiryReport.py</t>
-  </si>
-  <si>
     <t>Pharmacy\Reports\Stock\TC04NarcoticStockReport.py</t>
   </si>
   <si>
@@ -381,9 +333,6 @@
     <t>Reports\TC001BillingDashboardSummary.py</t>
   </si>
   <si>
-    <t>TC046</t>
-  </si>
-  <si>
     <t>TC047</t>
   </si>
   <si>
@@ -409,22 +358,13 @@
   </si>
   <si>
     <t>TC055</t>
-  </si>
-  <si>
-    <t>EMR-4700</t>
-  </si>
-  <si>
-    <t>Enhancement on billing Dashboard</t>
-  </si>
-  <si>
-    <t>Need Scripting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -440,16 +380,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,12 +391,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -509,8 +435,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -792,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G21" sqref="F21:G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,19 +745,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -841,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -855,7 +779,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -863,7 +787,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>4</v>
@@ -883,7 +807,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -900,10 +824,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>4</v>
@@ -920,10 +844,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -940,10 +864,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>4</v>
@@ -954,22 +878,16 @@
       <c r="E7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>4</v>
@@ -980,22 +898,16 @@
       <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -1006,22 +918,16 @@
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>4</v>
@@ -1038,10 +944,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>4</v>
@@ -1053,19 +959,15 @@
         <v>16</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>97</v>
-      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>4</v>
@@ -1082,10 +984,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>4</v>
@@ -1102,10 +1004,10 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>4</v>
@@ -1122,10 +1024,10 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>4</v>
@@ -1142,10 +1044,10 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>4</v>
@@ -1154,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1162,10 +1064,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>4</v>
@@ -1178,25 +1080,23 @@
       </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1204,10 +1104,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>4</v>
@@ -1227,7 +1127,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>4</v>
@@ -1247,7 +1147,7 @@
         <v>23</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>4</v>
@@ -1256,20 +1156,18 @@
         <v>0</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4" t="s">
-        <v>91</v>
-      </c>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>4</v>
@@ -1289,7 +1187,7 @@
         <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>4</v>
@@ -1298,20 +1196,18 @@
         <v>0</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4" t="s">
-        <v>92</v>
-      </c>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>4</v>
@@ -1328,10 +1224,10 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>4</v>
@@ -1348,10 +1244,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>4</v>
@@ -1368,10 +1264,10 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>4</v>
@@ -1391,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>4</v>
@@ -1408,10 +1304,10 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1420,7 +1316,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1428,10 +1324,10 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>4</v>
@@ -1440,7 +1336,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
@@ -1448,10 +1344,10 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>4</v>
@@ -1460,7 +1356,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
@@ -1468,10 +1364,10 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>4</v>
@@ -1480,18 +1376,18 @@
         <v>0</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>109</v>
+      <c r="A33" s="6" t="s">
+        <v>95</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>4</v>
@@ -1500,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
@@ -1508,10 +1404,10 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>4</v>
@@ -1527,11 +1423,11 @@
       <c r="H34" s="4"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
-        <v>110</v>
+      <c r="A35" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>4</v>
@@ -1540,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
@@ -1548,10 +1444,10 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>4</v>
@@ -1560,7 +1456,7 @@
         <v>0</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -1568,10 +1464,10 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>4</v>
@@ -1580,20 +1476,18 @@
         <v>0</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
-      <c r="H37" s="4" t="s">
-        <v>132</v>
-      </c>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>4</v>
@@ -1602,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -1610,10 +1504,10 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>4</v>
@@ -1622,7 +1516,7 @@
         <v>0</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
@@ -1630,10 +1524,10 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>4</v>
@@ -1642,7 +1536,7 @@
         <v>0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -1650,10 +1544,10 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>115</v>
+        <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>4</v>
@@ -1662,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
@@ -1670,10 +1564,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>4</v>
@@ -1682,7 +1576,7 @@
         <v>0</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
@@ -1690,10 +1584,10 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>4</v>
@@ -1702,7 +1596,7 @@
         <v>0</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
@@ -1710,10 +1604,10 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>4</v>
@@ -1722,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
@@ -1730,10 +1624,10 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>4</v>
@@ -1742,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
@@ -1750,10 +1644,10 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>4</v>
@@ -1762,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>61</v>
+        <v>106</v>
       </c>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
@@ -1770,10 +1664,10 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>102</v>
+        <v>42</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>4</v>
@@ -1782,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
@@ -1790,10 +1684,10 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>4</v>
@@ -1802,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
@@ -1810,10 +1704,10 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>4</v>
@@ -1822,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1830,10 +1724,10 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>4</v>
@@ -1842,22 +1736,18 @@
         <v>0</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="H50" s="4" t="s">
-        <v>131</v>
-      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>4</v>
@@ -1866,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
@@ -1874,10 +1764,10 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>4</v>
@@ -1886,95 +1776,11 @@
         <v>0</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="F52" s="4"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="4">
-        <v>0</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D54" s="4">
-        <v>0</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="4">
-        <v>0</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F55" s="4"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D56" s="4">
-        <v>0</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>